<commit_message>
dp and binary tree
</commit_message>
<xml_diff>
--- a/DSA_questions.xlsx
+++ b/DSA_questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F791F783-C85F-49E9-9050-9DA0C3017ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF952EF-0480-49F1-8385-5504B781BE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1903,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A408" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E416" sqref="E416"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="15.5"/>
@@ -3526,8 +3526,8 @@
       <c r="B156" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C156" s="16" t="s">
-        <v>468</v>
+      <c r="C156" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">
@@ -3537,8 +3537,8 @@
       <c r="B157" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C157" s="16" t="s">
-        <v>468</v>
+      <c r="C157" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21">
@@ -3548,8 +3548,8 @@
       <c r="B158" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C158" s="16" t="s">
-        <v>468</v>
+      <c r="C158" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3559,8 +3559,8 @@
       <c r="B159" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C159" s="16" t="s">
-        <v>468</v>
+      <c r="C159" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">
@@ -3570,8 +3570,8 @@
       <c r="B160" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C160" s="16" t="s">
-        <v>468</v>
+      <c r="C160" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
@@ -3581,8 +3581,8 @@
       <c r="B161" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C161" s="16" t="s">
-        <v>468</v>
+      <c r="C161" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">
@@ -3592,8 +3592,8 @@
       <c r="B162" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C162" s="16" t="s">
-        <v>468</v>
+      <c r="C162" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">
@@ -3603,8 +3603,8 @@
       <c r="B163" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C163" s="16" t="s">
-        <v>468</v>
+      <c r="C163" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
@@ -3614,8 +3614,8 @@
       <c r="B164" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C164" s="16" t="s">
-        <v>468</v>
+      <c r="C164" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21">
@@ -3625,8 +3625,8 @@
       <c r="B165" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C165" s="16" t="s">
-        <v>468</v>
+      <c r="C165" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="21">
@@ -3739,8 +3739,8 @@
       <c r="B177" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C177" s="4" t="s">
-        <v>3</v>
+      <c r="C177" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3750,8 +3750,8 @@
       <c r="B178" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>3</v>
+      <c r="C178" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3761,8 +3761,8 @@
       <c r="B179" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C179" s="4" t="s">
-        <v>3</v>
+      <c r="C179" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3772,8 +3772,8 @@
       <c r="B180" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C180" s="4" t="s">
-        <v>3</v>
+      <c r="C180" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -5626,8 +5626,8 @@
       <c r="B356" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C356" s="4" t="s">
-        <v>3</v>
+      <c r="C356" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">
@@ -5637,8 +5637,8 @@
       <c r="B357" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C357" s="4" t="s">
-        <v>3</v>
+      <c r="C357" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5659,8 +5659,8 @@
       <c r="B359" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C359" s="4" t="s">
-        <v>3</v>
+      <c r="C359" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">
@@ -6214,8 +6214,8 @@
       <c r="B412" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="C412" s="4" t="s">
-        <v>3</v>
+      <c r="C412" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6258,8 +6258,8 @@
       <c r="B416" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="C416" s="4" t="s">
-        <v>3</v>
+      <c r="C416" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="21">
@@ -6280,8 +6280,8 @@
       <c r="B418" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="C418" s="4" t="s">
-        <v>3</v>
+      <c r="C418" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="21">
@@ -6291,8 +6291,8 @@
       <c r="B419" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="C419" s="4" t="s">
-        <v>3</v>
+      <c r="C419" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">
@@ -6588,8 +6588,8 @@
       <c r="B446" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="C446" s="4" t="s">
-        <v>3</v>
+      <c r="C446" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="21">
@@ -6599,8 +6599,8 @@
       <c r="B447" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="C447" s="4" t="s">
-        <v>3</v>
+      <c r="C447" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="448" spans="1:3" ht="21">
@@ -6863,8 +6863,8 @@
       <c r="B472" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="C472" s="4" t="s">
-        <v>3</v>
+      <c r="C472" s="12" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">

</xml_diff>